<commit_message>
added first set of RF scores
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\Desktop\Classwork\Final Project\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C177DE2-347B-4510-80A2-265EEA941F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A61807-F841-4B86-BB06-707C06CAD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="18">
   <si>
     <t>Dataset</t>
   </si>
@@ -78,14 +78,34 @@
   </si>
   <si>
     <t>SMOTEENN</t>
+  </si>
+  <si>
+    <t>F1 = 0.80 / 0.82</t>
+  </si>
+  <si>
+    <t>F1 = 0.82 /0.82</t>
+  </si>
+  <si>
+    <t>Unscaled</t>
+  </si>
+  <si>
+    <t>F1 = 0.83 / 0.83</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,12 +129,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA3959B-2C30-46C0-8811-DAD31D9C9BA3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,47 +477,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -495,42 +534,51 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -538,34 +586,34 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -573,6 +621,14 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -870,7 +926,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE27B2-7D78-4FE4-91C8-C360C29011FD}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,130 +1077,151 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Model Best Results Record.xlsx
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\Desktop\Classwork\Final Project\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B4CF63-C642-4B2C-9012-71E4EB06C88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCBA2DF-78EE-425E-BC70-28BDAB4A4E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="1695" yWindow="1965" windowWidth="15375" windowHeight="7965" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="21">
   <si>
     <t>Dataset</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>F1 = 0.97 / 0.61</t>
+  </si>
+  <si>
+    <t>F1= 0.98/.00</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,6 +567,9 @@
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
jason adding logre model results
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\Desktop\Classwork\Final Project\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonm/Desktop/Stroke/GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6593291D-1971-44B3-8953-57EEE361EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124EDE7F-4439-FC40-9330-39A6DBD3B94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="22">
   <si>
     <t>Dataset</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>F1 = 0.94 / 0.24</t>
+  </si>
+  <si>
+    <t>F1 = 0.84 / 0.85</t>
+  </si>
+  <si>
+    <t>F1 = 0.82/ 0.21</t>
   </si>
 </sst>
 </file>
@@ -468,21 +474,21 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -518,8 +524,11 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -529,8 +538,11 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -540,8 +552,11 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -551,8 +566,11 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -565,8 +583,11 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -575,6 +596,9 @@
       </c>
       <c r="E7" t="s">
         <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -590,20 +614,20 @@
       <selection activeCell="F1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -614,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -625,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -633,7 +657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -641,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -649,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -660,7 +684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -668,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -676,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -684,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -695,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -703,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -711,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -732,20 +756,20 @@
       <selection activeCell="E1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -756,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -767,7 +791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -775,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -783,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -791,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -802,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -810,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -818,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -826,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -837,7 +861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -845,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -853,7 +877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -874,20 +898,20 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -898,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -909,7 +933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -917,7 +941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -925,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -933,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -944,7 +968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -952,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -960,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -968,7 +992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -979,7 +1003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -987,7 +1011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -995,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1016,18 +1040,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1068,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -1071,7 +1095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1079,7 +1103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1095,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -1122,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1130,7 +1154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Revert "adding additional models"
This reverts commit 9e76aa3ff031131123fea082964002e6e6d01975.
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonm/Desktop/Stroke/GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C177DE2-347B-4510-80A2-265EEA941F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124EDE7F-4439-FC40-9330-39A6DBD3B94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="22">
   <si>
     <t>Dataset</t>
   </si>
@@ -78,14 +78,46 @@
   </si>
   <si>
     <t>SMOTEENN</t>
+  </si>
+  <si>
+    <t>F1 = 0.80 / 0.82</t>
+  </si>
+  <si>
+    <t>F1 = 0.82 /0.82</t>
+  </si>
+  <si>
+    <t>Unscaled</t>
+  </si>
+  <si>
+    <t>F1 = 0.83 / 0.83</t>
+  </si>
+  <si>
+    <t>F1 = 0.93 / 0.24</t>
+  </si>
+  <si>
+    <t>F1 = 0.94 / 0.24</t>
+  </si>
+  <si>
+    <t>F1 = 0.84 / 0.85</t>
+  </si>
+  <si>
+    <t>F1 = 0.82/ 0.21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,12 +141,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,151 +471,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA3959B-2C30-46C0-8811-DAD31D9C9BA3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -589,20 +614,20 @@
       <selection activeCell="F1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -613,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -624,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -632,7 +657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -640,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -648,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -659,7 +684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -667,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -675,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -683,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -694,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -702,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -710,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -731,20 +756,20 @@
       <selection activeCell="E1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -755,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -766,7 +791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -774,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -782,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -790,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -801,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -809,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -817,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -825,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -836,7 +861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -844,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -852,7 +877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -870,23 +895,23 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -897,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -908,7 +933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -916,7 +941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -924,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -932,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -943,7 +968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -951,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -959,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -967,7 +992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -978,7 +1003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -986,7 +1011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -994,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1009,142 +1034,163 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE27B2-7D78-4FE4-91C8-C360C29011FD}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "adding additional models""
This reverts commit f962606fb61db93f7912fdf8961a56fe0791c1c2.
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonm/Desktop/Stroke/GroupProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124EDE7F-4439-FC40-9330-39A6DBD3B94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C177DE2-347B-4510-80A2-265EEA941F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="14">
   <si>
     <t>Dataset</t>
   </si>
@@ -78,46 +78,14 @@
   </si>
   <si>
     <t>SMOTEENN</t>
-  </si>
-  <si>
-    <t>F1 = 0.80 / 0.82</t>
-  </si>
-  <si>
-    <t>F1 = 0.82 /0.82</t>
-  </si>
-  <si>
-    <t>Unscaled</t>
-  </si>
-  <si>
-    <t>F1 = 0.83 / 0.83</t>
-  </si>
-  <si>
-    <t>F1 = 0.93 / 0.24</t>
-  </si>
-  <si>
-    <t>F1 = 0.94 / 0.24</t>
-  </si>
-  <si>
-    <t>F1 = 0.84 / 0.85</t>
-  </si>
-  <si>
-    <t>F1 = 0.82/ 0.21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -141,22 +109,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,134 +429,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA3959B-2C30-46C0-8811-DAD31D9C9BA3}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -614,20 +589,20 @@
       <selection activeCell="F1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -638,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -649,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -657,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -665,7 +640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -673,7 +648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -684,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -692,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -700,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -708,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -719,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -727,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -735,7 +710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -756,20 +731,20 @@
       <selection activeCell="E1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -791,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -799,7 +774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -807,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -815,7 +790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -826,7 +801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -834,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -842,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -850,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -861,7 +836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -869,7 +844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -877,7 +852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -895,23 +870,23 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -922,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -933,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -941,7 +916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -949,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -957,7 +932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -968,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -976,7 +951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -984,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -992,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1003,7 +978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1011,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1034,163 +1009,142 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE27B2-7D78-4FE4-91C8-C360C29011FD}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with best NN model
</commit_message>
<xml_diff>
--- a/Model Best Results Record.xlsx
+++ b/Model Best Results Record.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Documents\GitHub\GroupProject\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCBA2DF-78EE-425E-BC70-28BDAB4A4E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12935B39-AA45-40BD-9D4B-48C60D4C8EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="1965" windowWidth="15375" windowHeight="7965" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6C275FEE-6EC3-42A7-97A7-2182124BAA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="37">
   <si>
     <t>Dataset</t>
   </si>
@@ -99,13 +99,61 @@
   </si>
   <si>
     <t>F1= 0.98/.00</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Balanced</t>
+  </si>
+  <si>
+    <t>.50 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>1.0 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>0.67 &amp; 0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanced </t>
+  </si>
+  <si>
+    <t>Scaled</t>
+  </si>
+  <si>
+    <t>.67 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>.96 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>.98 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>0.98 &amp; 0.0</t>
+  </si>
+  <si>
+    <t>F1 = 0.67 / 0.0</t>
+  </si>
+  <si>
+    <t>F1 = 0.98 / 0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +169,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -147,13 +202,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +538,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +585,9 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
@@ -528,6 +598,9 @@
       </c>
       <c r="C3" t="s">
         <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -540,6 +613,9 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
@@ -551,6 +627,9 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
@@ -565,6 +644,9 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
@@ -578,6 +660,9 @@
       </c>
       <c r="C7" t="s">
         <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1016,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE27B2-7D78-4FE4-91C8-C360C29011FD}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,15 +1119,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1050,74 +1129,167 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>0.79759999999999998</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>0.79759999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>0.84519999999999995</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>0.95722700000000005</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>0.95652199999999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>0.95652099999999995</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,50 +1297,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>0.95652099999999995</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>